<commit_message>
Veranderingen maar weet niet meer wat :)
</commit_message>
<xml_diff>
--- a/Lasten.xlsx
+++ b/Lasten.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\School\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian Dibbets\Documents\School\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="19524"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="38400" windowHeight="19530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Juni" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="54">
   <si>
     <t>Discord</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Pin</t>
+  </si>
+  <si>
+    <t>Leon kermis</t>
+  </si>
+  <si>
+    <t>Deen</t>
+  </si>
+  <si>
+    <t>Broer Zondag</t>
+  </si>
+  <si>
+    <t>Broer zondag</t>
+  </si>
+  <si>
+    <t>Kleding geld</t>
   </si>
 </sst>
 </file>
@@ -333,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -349,6 +364,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -666,22 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -692,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>4.99</v>
       </c>
@@ -715,7 +731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>0.83333333333333337</v>
       </c>
@@ -738,7 +754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3.99</v>
       </c>
@@ -761,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>24.5</v>
       </c>
@@ -784,7 +800,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>9.99</v>
       </c>
@@ -807,7 +823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>13.99</v>
       </c>
@@ -827,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="12">
         <f>SUM(1.75, 1.8, 0.7, 0.7)</f>
         <v>4.95</v>
@@ -842,7 +858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="12">
         <v>32.82</v>
       </c>
@@ -856,7 +872,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="12">
         <v>14.65</v>
       </c>
@@ -870,7 +886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="12">
         <v>8.5500000000000007</v>
       </c>
@@ -884,15 +900,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="12">
         <v>8.8000000000000007</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="12">
         <f>SUM(26.1, 5.25)</f>
         <v>31.35</v>
@@ -901,7 +920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="12">
         <v>8.83</v>
       </c>
@@ -909,7 +928,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="12">
         <v>9.6</v>
       </c>
@@ -917,7 +936,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="12">
         <v>10</v>
       </c>
@@ -925,7 +944,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="12">
         <v>11.34</v>
       </c>
@@ -933,7 +952,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="12">
         <v>2.39</v>
       </c>
@@ -941,7 +960,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="12">
         <v>12.75</v>
       </c>
@@ -949,7 +968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="12">
         <v>7.5</v>
       </c>
@@ -957,12 +976,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="12">
         <v>6.95</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="12">
         <v>30</v>
       </c>
@@ -970,12 +989,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="12">
         <v>4.47</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>13</v>
       </c>
@@ -983,16 +1007,16 @@
         <v>14.44</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="12">
         <f>SUM(E2:E17)</f>
-        <v>496</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>11</v>
       </c>
@@ -1001,27 +1025,30 @@
         <v>58.293333333333337</v>
       </c>
     </row>
-    <row r="28" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="12">
         <f>SUM(C2:C100)</f>
-        <v>342.09</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>373.09</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="13">
         <f>SUM(E25:E26)-(E27)-(E28)</f>
-        <v>110.05666666666667</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>110.05666666666673</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>14</v>
+      </c>
+      <c r="E30" s="12">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1044,16 +1071,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -1066,71 +1093,93 @@
         <v>7</v>
       </c>
       <c r="F1" s="8"/>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3" s="2">
+        <v>14.71</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="15">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -1142,7 +1191,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -1154,7 +1203,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -1166,7 +1215,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1174,7 +1223,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1182,7 +1231,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -1190,7 +1239,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -1198,7 +1247,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -1206,7 +1255,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -1214,7 +1263,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -1222,7 +1271,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -1230,7 +1279,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -1238,12 +1287,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -1251,10 +1300,10 @@
       </c>
       <c r="E19" s="10">
         <f>Juni!E30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -1262,10 +1311,10 @@
       </c>
       <c r="E20" s="10">
         <f>SUM(E2:E17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -1276,7 +1325,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -1284,10 +1333,10 @@
       </c>
       <c r="E22" s="10">
         <f>SUM(C2:C17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>132.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -1295,10 +1344,10 @@
       </c>
       <c r="E23" s="10">
         <f>SUM(E19:E20)-(E21)-(E22)</f>
-        <v>-83.283333333333317</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>74.206666666666706</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
@@ -1327,12 +1376,12 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -1349,7 +1398,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
@@ -1364,7 +1413,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
@@ -1379,7 +1428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -1394,7 +1443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
@@ -1409,7 +1458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -1421,7 +1470,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -1433,7 +1482,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -1445,7 +1494,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1453,7 +1502,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1461,7 +1510,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -1469,7 +1518,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -1477,7 +1526,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -1485,7 +1534,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -1493,7 +1542,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -1501,7 +1550,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -1509,7 +1558,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -1517,12 +1566,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -1533,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -1544,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -1555,7 +1604,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -1566,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -1577,7 +1626,7 @@
         <v>-83.283333333333317</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
@@ -1606,12 +1655,12 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -1628,7 +1677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
@@ -1643,7 +1692,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
@@ -1658,7 +1707,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -1673,7 +1722,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
@@ -1688,7 +1737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -1700,7 +1749,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -1712,7 +1761,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -1724,7 +1773,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1732,7 +1781,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1740,7 +1789,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -1748,7 +1797,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -1756,7 +1805,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -1764,7 +1813,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -1772,7 +1821,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -1780,7 +1829,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -1788,7 +1837,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -1796,12 +1845,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -1812,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -1823,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -1834,7 +1883,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -1845,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -1856,7 +1905,7 @@
         <v>-83.283333333333317</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
@@ -1885,12 +1934,12 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -1907,7 +1956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
@@ -1922,7 +1971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
@@ -1937,7 +1986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -1952,7 +2001,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
@@ -1967,7 +2016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -1979,7 +2028,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -1991,7 +2040,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -2003,7 +2052,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -2011,7 +2060,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -2019,7 +2068,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -2027,7 +2076,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -2035,7 +2084,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -2043,7 +2092,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -2051,7 +2100,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -2059,7 +2108,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -2067,7 +2116,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -2075,12 +2124,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -2091,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -2102,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -2113,7 +2162,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -2124,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -2135,7 +2184,7 @@
         <v>-83.283333333333317</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
@@ -2164,12 +2213,12 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -2186,7 +2235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
@@ -2201,7 +2250,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
@@ -2216,7 +2265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -2231,7 +2280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
@@ -2246,7 +2295,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -2258,7 +2307,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -2270,7 +2319,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -2282,7 +2331,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -2290,7 +2339,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -2298,7 +2347,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -2306,7 +2355,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -2314,7 +2363,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -2322,7 +2371,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -2330,7 +2379,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -2338,7 +2387,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -2346,7 +2395,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -2354,12 +2403,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -2370,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -2381,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -2392,7 +2441,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -2403,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -2414,7 +2463,7 @@
         <v>-83.283333333333317</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
@@ -2443,12 +2492,12 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -2465,7 +2514,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4.99</v>
       </c>
@@ -2480,7 +2529,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>24.99</v>
       </c>
@@ -2495,7 +2544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -2510,7 +2559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3.99</v>
       </c>
@@ -2525,7 +2574,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>24.5</v>
       </c>
@@ -2537,7 +2586,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.99</v>
       </c>
@@ -2549,7 +2598,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>13.99</v>
       </c>
@@ -2561,7 +2610,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -2569,7 +2618,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -2577,7 +2626,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -2585,7 +2634,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -2593,7 +2642,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -2601,7 +2650,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
@@ -2609,7 +2658,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -2617,7 +2666,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -2625,7 +2674,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -2633,12 +2682,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="9" t="s">
@@ -2649,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="s">
@@ -2660,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="9" t="s">
@@ -2671,7 +2720,7 @@
         <v>83.283333333333317</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="9" t="s">
@@ -2682,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="9" t="s">
@@ -2693,33 +2742,33 @@
         <v>-83.283333333333317</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" s="11"/>
       <c r="E32" s="6"/>
     </row>
@@ -2756,21 +2805,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="25.6640625" customWidth="1"/>
+    <col min="1" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="1">
         <f>SUM(Juni!E26,Juli!E20,Augustus!E20,September!E20,Oktober!E20,November!E20,December!E20)</f>
-        <v>496</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2779,22 +2828,22 @@
         <v>557.99333333333323</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="1">
         <f>SUM(Juni!E28,Juli!E22,Augustus!E22,September!E22,Oktober!E22,November!E22,December!E22)</f>
-        <v>342.09</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>505.59999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B1-B2-B3</f>
-        <v>-404.0833333333332</v>
+        <v>-326.59333333333319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>